<commit_message>
Sheets are different for ST-10 and VF-2
</commit_message>
<xml_diff>
--- a/DB Table columns.xlsx
+++ b/DB Table columns.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Static" sheetId="1" r:id="rId1"/>
-    <sheet name="Variable" sheetId="2" r:id="rId2"/>
+    <sheet name="VF-2 Variables" sheetId="3" r:id="rId2"/>
+    <sheet name="ST-10 Variables" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="132">
   <si>
     <t>Machine Serial Number</t>
   </si>
@@ -758,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1315,4 +1316,440 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Publishing now is only if anything except time has changed
</commit_message>
<xml_diff>
--- a/DB Table columns.xlsx
+++ b/DB Table columns.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Static" sheetId="1" r:id="rId1"/>
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add datatypes to rows
</commit_message>
<xml_diff>
--- a/DB Table columns.xlsx
+++ b/DB Table columns.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Static" sheetId="1" r:id="rId1"/>
-    <sheet name="VF-2 Variables" sheetId="3" r:id="rId2"/>
-    <sheet name="ST-10 Variables" sheetId="2" r:id="rId3"/>
+    <sheet name="Variable" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="130">
   <si>
     <t>Machine Serial Number</t>
   </si>
@@ -137,9 +136,6 @@
     <t>Override [FEED HOLD] control</t>
   </si>
   <si>
-    <t>Programmable stop with message</t>
-  </si>
-  <si>
     <t>Year, month, day</t>
   </si>
   <si>
@@ -276,9 +272,6 @@
   </si>
   <si>
     <t>?Q600 3004</t>
-  </si>
-  <si>
-    <t>?Q600 3006</t>
   </si>
   <si>
     <t>?Q600 3011</t>
@@ -759,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,46 +764,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
-        <v>59</v>
-      </c>
       <c r="C1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -820,10 +813,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,144 +827,144 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="C1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
@@ -979,7 +972,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -987,7 +980,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -995,7 +988,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
@@ -1003,7 +996,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
@@ -1011,7 +1004,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
@@ -1019,7 +1012,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
@@ -1027,7 +1020,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
@@ -1035,7 +1028,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -1043,7 +1036,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
@@ -1051,7 +1044,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
@@ -1059,7 +1052,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
@@ -1067,7 +1060,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
@@ -1075,7 +1068,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
@@ -1083,7 +1076,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
@@ -1091,7 +1084,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
@@ -1099,7 +1092,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
@@ -1107,7 +1100,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
@@ -1115,7 +1108,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
@@ -1123,7 +1116,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
@@ -1131,7 +1124,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
@@ -1139,7 +1132,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B35" t="s">
         <v>34</v>
@@ -1147,7 +1140,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
@@ -1155,7 +1148,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
@@ -1163,7 +1156,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B38" t="s">
         <v>37</v>
@@ -1171,15 +1164,15 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
@@ -1187,7 +1180,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B41" t="s">
         <v>42</v>
@@ -1195,7 +1188,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" t="s">
         <v>43</v>
@@ -1203,7 +1196,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B43" t="s">
         <v>44</v>
@@ -1211,7 +1204,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B44" t="s">
         <v>45</v>
@@ -1219,7 +1212,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B45" t="s">
         <v>46</v>
@@ -1227,7 +1220,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
@@ -1235,7 +1228,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B47" t="s">
         <v>48</v>
@@ -1243,7 +1236,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
         <v>49</v>
@@ -1251,7 +1244,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
         <v>50</v>
@@ -1259,7 +1252,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B50" t="s">
         <v>51</v>
@@ -1267,7 +1260,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B51" t="s">
         <v>52</v>
@@ -1275,7 +1268,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B52" t="s">
         <v>53</v>
@@ -1283,7 +1276,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B53" t="s">
         <v>54</v>
@@ -1291,7 +1284,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B54" t="s">
         <v>55</v>
@@ -1299,454 +1292,10 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B55" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>104</v>
-      </c>
-      <c r="B56" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C48"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>73</v>
-      </c>
-      <c r="B27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>85</v>
-      </c>
-      <c r="B31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>89</v>
-      </c>
-      <c r="B33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>90</v>
-      </c>
-      <c r="B34" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>93</v>
-      </c>
-      <c r="B37" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>95</v>
-      </c>
-      <c r="B39" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>96</v>
-      </c>
-      <c r="B40" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>98</v>
-      </c>
-      <c r="B42" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>99</v>
-      </c>
-      <c r="B43" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>100</v>
-      </c>
-      <c r="B44" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>101</v>
-      </c>
-      <c r="B45" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>102</v>
-      </c>
-      <c r="B46" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>103</v>
-      </c>
-      <c r="B47" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>104</v>
-      </c>
-      <c r="B48" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change in datatypes and number of parameters
</commit_message>
<xml_diff>
--- a/DB Table columns.xlsx
+++ b/DB Table columns.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Static" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="116">
   <si>
     <t>Machine Serial Number</t>
   </si>
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37:C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,7 +1201,7 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1212,7 +1212,7 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1223,7 +1223,7 @@
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1234,7 +1234,7 @@
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1245,7 +1245,7 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1256,7 +1256,7 @@
         <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1367,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37:C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,7 +1793,7 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1804,7 +1804,7 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1815,7 +1815,7 @@
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1826,7 +1826,7 @@
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1837,7 +1837,7 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1848,7 +1848,7 @@
         <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1968,10 +1968,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2285,7 +2285,7 @@
         <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2296,7 +2296,7 @@
         <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2307,7 +2307,7 @@
         <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2318,7 +2318,7 @@
         <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2329,7 +2329,7 @@
         <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2340,7 +2340,7 @@
         <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2411,24 +2411,17 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C40" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>98</v>
-      </c>
-      <c r="B41" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes to the table's variables
</commit_message>
<xml_diff>
--- a/DB Table columns.xlsx
+++ b/DB Table columns.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Static" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="116">
   <si>
     <t>Machine Serial Number</t>
   </si>
@@ -1367,7 +1367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C37" sqref="C37:C43"/>
     </sheetView>
   </sheetViews>
@@ -1968,10 +1968,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,10 +2136,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
         <v>115</v>
@@ -2147,10 +2147,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>115</v>
@@ -2158,10 +2158,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
         <v>115</v>
@@ -2169,10 +2169,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
         <v>115</v>
@@ -2180,10 +2180,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
         <v>115</v>
@@ -2191,10 +2191,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
         <v>115</v>
@@ -2202,10 +2202,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
         <v>115</v>
@@ -2213,10 +2213,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
         <v>115</v>
@@ -2224,10 +2224,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
         <v>115</v>
@@ -2235,10 +2235,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
         <v>115</v>
@@ -2246,10 +2246,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
         <v>115</v>
@@ -2257,10 +2257,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
         <v>115</v>
@@ -2268,10 +2268,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
         <v>115</v>
@@ -2279,10 +2279,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
         <v>115</v>
@@ -2290,10 +2290,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
         <v>115</v>
@@ -2301,10 +2301,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
         <v>115</v>
@@ -2312,10 +2312,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
         <v>115</v>
@@ -2323,10 +2323,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
         <v>115</v>
@@ -2334,32 +2334,32 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
         <v>115</v>
@@ -2367,10 +2367,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C36" t="s">
         <v>115</v>
@@ -2378,10 +2378,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C37" t="s">
         <v>115</v>
@@ -2389,10 +2389,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C38" t="s">
         <v>115</v>
@@ -2400,23 +2400,12 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C39" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>98</v>
-      </c>
-      <c r="B40" t="s">
-        <v>54</v>
-      </c>
-      <c r="C40" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>